<commit_message>
made df of each filetypes
</commit_message>
<xml_diff>
--- a/data/WordTimeSeries.xlsx
+++ b/data/WordTimeSeries.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sano/Dropbox/Work/20200327_COVIT19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keigo/twitter-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25C025B-1BDC-9644-BB0B-452EED120585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E6134C-27D0-9441-AE9E-D2B364396939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="3560" windowWidth="27900" windowHeight="16940" xr2:uid="{8C09E5C1-39D7-E74D-9E20-BE6DEF00F715}"/>
+    <workbookView xWindow="2940" yWindow="3680" windowWidth="27900" windowHeight="16940" xr2:uid="{8C09E5C1-39D7-E74D-9E20-BE6DEF00F715}"/>
   </bookViews>
   <sheets>
     <sheet name="Word List" sheetId="1" r:id="rId1"/>
-    <sheet name="Tension" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Word List'!$C$2:$C$48</definedName>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="424">
   <si>
     <t>file name</t>
     <phoneticPr fontId="1"/>
@@ -1613,20 +1612,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="164" formatCode="0_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1652,16 +1651,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1677,7 +1675,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1978,24 +1976,24 @@
   </sheetPr>
   <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="K146" sqref="K146"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="F151" sqref="F136:F151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2020,7 +2018,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -2031,7 +2029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>417</v>
       </c>
@@ -2042,7 +2040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -2053,7 +2051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2064,7 +2062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>418</v>
       </c>
@@ -2075,7 +2073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2086,7 +2084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -2097,7 +2095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>419</v>
       </c>
@@ -2108,7 +2106,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>420</v>
       </c>
@@ -2119,7 +2117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>421</v>
       </c>
@@ -2130,7 +2128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>422</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
@@ -2152,7 +2150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>32</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>37</v>
       </c>
@@ -2185,7 +2183,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
@@ -2196,7 +2194,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>43</v>
       </c>
@@ -2207,7 +2205,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>46</v>
       </c>
@@ -2218,7 +2216,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>49</v>
       </c>
@@ -2229,7 +2227,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2240,7 +2238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2254,7 +2252,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
@@ -2265,7 +2263,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>64</v>
       </c>
@@ -2276,7 +2274,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
@@ -2287,7 +2285,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
@@ -2298,7 +2296,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>73</v>
       </c>
@@ -2309,7 +2307,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
@@ -2320,7 +2318,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
@@ -2331,7 +2329,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
@@ -2342,7 +2340,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
@@ -2353,7 +2351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
@@ -2364,7 +2362,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>89</v>
       </c>
@@ -2375,7 +2373,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>92</v>
       </c>
@@ -2386,7 +2384,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>95</v>
       </c>
@@ -2397,7 +2395,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>97</v>
       </c>
@@ -2408,7 +2406,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>100</v>
       </c>
@@ -2419,7 +2417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>102</v>
       </c>
@@ -2430,7 +2428,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>105</v>
       </c>
@@ -2441,7 +2439,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>108</v>
       </c>
@@ -2452,7 +2450,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>111</v>
       </c>
@@ -2463,7 +2461,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>114</v>
       </c>
@@ -2474,7 +2472,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>117</v>
       </c>
@@ -2485,7 +2483,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>120</v>
       </c>
@@ -2496,7 +2494,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>122</v>
       </c>
@@ -2507,7 +2505,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>124</v>
       </c>
@@ -2518,7 +2516,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>126</v>
       </c>
@@ -2532,7 +2530,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>130</v>
       </c>
@@ -2543,7 +2541,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>133</v>
       </c>
@@ -2554,7 +2552,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>136</v>
       </c>
@@ -2565,7 +2563,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>139</v>
       </c>
@@ -2576,7 +2574,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>142</v>
       </c>
@@ -2587,7 +2585,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>145</v>
       </c>
@@ -2598,7 +2596,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>148</v>
       </c>
@@ -2609,7 +2607,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>151</v>
       </c>
@@ -2620,7 +2618,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>154</v>
       </c>
@@ -2631,7 +2629,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>157</v>
       </c>
@@ -2642,7 +2640,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>163</v>
       </c>
@@ -2664,7 +2662,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>165</v>
       </c>
@@ -2675,7 +2673,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>168</v>
       </c>
@@ -2686,7 +2684,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>171</v>
       </c>
@@ -2697,7 +2695,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>174</v>
       </c>
@@ -2708,7 +2706,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>177</v>
       </c>
@@ -2719,7 +2717,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>180</v>
       </c>
@@ -2730,7 +2728,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>183</v>
       </c>
@@ -2741,7 +2739,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>186</v>
       </c>
@@ -2752,7 +2750,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>189</v>
       </c>
@@ -2763,7 +2761,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>192</v>
       </c>
@@ -2774,7 +2772,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>194</v>
       </c>
@@ -2785,7 +2783,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>197</v>
       </c>
@@ -2796,7 +2794,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -2810,7 +2808,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>204</v>
       </c>
@@ -2821,7 +2819,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>207</v>
       </c>
@@ -2832,7 +2830,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>210</v>
       </c>
@@ -2843,7 +2841,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>213</v>
       </c>
@@ -2854,7 +2852,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
         <v>216</v>
       </c>
@@ -2865,7 +2863,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>219</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
         <v>222</v>
       </c>
@@ -2887,7 +2885,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>225</v>
       </c>
@@ -2898,7 +2896,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>227</v>
       </c>
@@ -2909,7 +2907,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
         <v>230</v>
       </c>
@@ -2920,7 +2918,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="87" spans="2:4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
         <v>232</v>
       </c>
@@ -2931,7 +2929,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="2:4">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
         <v>235</v>
       </c>
@@ -2942,7 +2940,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="89" spans="2:4">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
         <v>237</v>
       </c>
@@ -2953,7 +2951,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="2:4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
         <v>240</v>
       </c>
@@ -2964,7 +2962,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="91" spans="2:4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="s">
         <v>242</v>
       </c>
@@ -2975,7 +2973,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="2:4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B92" s="1" t="s">
         <v>245</v>
       </c>
@@ -2986,7 +2984,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="93" spans="2:4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93" s="1" t="s">
         <v>248</v>
       </c>
@@ -2997,7 +2995,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="2:4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
         <v>423</v>
       </c>
@@ -3008,7 +3006,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="2:4">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" s="1" t="s">
         <v>252</v>
       </c>
@@ -3019,10 +3017,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="96" spans="2:4">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>255</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B98" s="1" t="s">
         <v>259</v>
       </c>
@@ -3047,7 +3045,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B99" s="1" t="s">
         <v>262</v>
       </c>
@@ -3058,7 +3056,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B100" s="1" t="s">
         <v>265</v>
       </c>
@@ -3069,7 +3067,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="s">
         <v>268</v>
       </c>
@@ -3080,7 +3078,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B102" s="1" t="s">
         <v>271</v>
       </c>
@@ -3091,7 +3089,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B103" s="1" t="s">
         <v>274</v>
       </c>
@@ -3102,7 +3100,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B104" s="1" t="s">
         <v>277</v>
       </c>
@@ -3113,7 +3111,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B105" s="1" t="s">
         <v>279</v>
       </c>
@@ -3124,7 +3122,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B106" s="1" t="s">
         <v>282</v>
       </c>
@@ -3135,7 +3133,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B107" s="1" t="s">
         <v>285</v>
       </c>
@@ -3146,7 +3144,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B108" s="1" t="s">
         <v>288</v>
       </c>
@@ -3157,7 +3155,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B109" s="1" t="s">
         <v>290</v>
       </c>
@@ -3168,7 +3166,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B110" s="1" t="s">
         <v>292</v>
       </c>
@@ -3179,7 +3177,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B111" s="1" t="s">
         <v>294</v>
       </c>
@@ -3190,7 +3188,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B112" s="1" t="s">
         <v>297</v>
       </c>
@@ -3201,7 +3199,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B113" s="1" t="s">
         <v>299</v>
       </c>
@@ -3212,7 +3210,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B114" s="1" t="s">
         <v>301</v>
       </c>
@@ -3223,7 +3221,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B115" s="1" t="s">
         <v>304</v>
       </c>
@@ -3234,7 +3232,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B116" s="1" t="s">
         <v>306</v>
       </c>
@@ -3245,7 +3243,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B117" s="1" t="s">
         <v>309</v>
       </c>
@@ -3256,7 +3254,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B118" s="1" t="s">
         <v>312</v>
       </c>
@@ -3267,7 +3265,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>315</v>
       </c>
@@ -3281,7 +3279,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B121" s="1" t="s">
         <v>319</v>
       </c>
@@ -3292,7 +3290,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B122" s="1" t="s">
         <v>322</v>
       </c>
@@ -3303,7 +3301,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B123" s="1" t="s">
         <v>325</v>
       </c>
@@ -3314,7 +3312,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B124" s="1" t="s">
         <v>328</v>
       </c>
@@ -3325,7 +3323,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B125" s="1" t="s">
         <v>331</v>
       </c>
@@ -3336,7 +3334,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B126" s="1" t="s">
         <v>334</v>
       </c>
@@ -3347,7 +3345,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B127" s="1" t="s">
         <v>337</v>
       </c>
@@ -3358,7 +3356,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B128" s="1" t="s">
         <v>340</v>
       </c>
@@ -3369,7 +3367,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="129" spans="2:4">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B129" s="1" t="s">
         <v>343</v>
       </c>
@@ -3380,7 +3378,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="130" spans="2:4">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B130" s="1" t="s">
         <v>346</v>
       </c>
@@ -3391,7 +3389,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="131" spans="2:4">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B131" s="1" t="s">
         <v>349</v>
       </c>
@@ -3402,7 +3400,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="132" spans="2:4">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B132" s="1" t="s">
         <v>352</v>
       </c>
@@ -3413,7 +3411,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="133" spans="2:4">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B133" s="1" t="s">
         <v>355</v>
       </c>
@@ -3424,7 +3422,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="134" spans="2:4">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B134" s="1" t="s">
         <v>358</v>
       </c>
@@ -3435,7 +3433,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="135" spans="2:4">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B135" s="1" t="s">
         <v>361</v>
       </c>
@@ -3446,7 +3444,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="136" spans="2:4">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B136" s="1" t="s">
         <v>364</v>
       </c>
@@ -3457,7 +3455,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="137" spans="2:4">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B137" s="1" t="s">
         <v>367</v>
       </c>
@@ -3468,7 +3466,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="138" spans="2:4">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B138" s="1" t="s">
         <v>370</v>
       </c>
@@ -3479,7 +3477,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="139" spans="2:4">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B139" s="1" t="s">
         <v>373</v>
       </c>
@@ -3490,7 +3488,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="140" spans="2:4">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B140" s="1" t="s">
         <v>376</v>
       </c>
@@ -3501,7 +3499,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="141" spans="2:4">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B141" s="1" t="s">
         <v>379</v>
       </c>
@@ -3512,7 +3510,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="142" spans="2:4">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B142" s="1" t="s">
         <v>382</v>
       </c>
@@ -3523,7 +3521,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="143" spans="2:4">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B143" s="1" t="s">
         <v>384</v>
       </c>
@@ -3534,7 +3532,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="144" spans="2:4">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="1" t="s">
         <v>387</v>
       </c>
@@ -3545,7 +3543,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="145" spans="2:4">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B145" s="1" t="s">
         <v>390</v>
       </c>
@@ -3556,7 +3554,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="146" spans="2:4">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="1" t="s">
         <v>393</v>
       </c>
@@ -3567,7 +3565,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="147" spans="2:4">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B147" s="1" t="s">
         <v>396</v>
       </c>
@@ -3578,7 +3576,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="148" spans="2:4">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B148" s="1" t="s">
         <v>399</v>
       </c>
@@ -3589,7 +3587,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="149" spans="2:4">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B149" s="1" t="s">
         <v>402</v>
       </c>
@@ -3600,7 +3598,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="150" spans="2:4">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B150" s="1" t="s">
         <v>405</v>
       </c>
@@ -3611,7 +3609,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="151" spans="2:4">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B151" s="1" t="s">
         <v>407</v>
       </c>
@@ -3622,7 +3620,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="152" spans="2:4">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="1" t="s">
         <v>410</v>
       </c>
@@ -3633,7 +3631,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="153" spans="2:4">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B153" s="1" t="s">
         <v>412</v>
       </c>
@@ -3644,7 +3642,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="154" spans="2:4">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B154" s="1" t="s">
         <v>415</v>
       </c>
@@ -3660,455 +3658,4 @@
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" scale="39" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF95232-2607-BB4A-B8F7-F8D98CF0CD49}">
-  <dimension ref="A1:V63"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>418</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="K2" t="s">
-        <v>420</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="M2" t="s">
-        <v>422</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="3">
-        <v>43862</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="3">
-        <v>43863</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="3">
-        <v>43864</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="3">
-        <v>43865</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="3">
-        <v>43866</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="3">
-        <v>43867</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="3">
-        <v>43868</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="3">
-        <v>43869</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="3">
-        <v>43870</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="3">
-        <v>43871</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="3">
-        <v>43872</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="3">
-        <v>43873</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="3">
-        <v>43874</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="3">
-        <v>43875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="3">
-        <v>43876</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="3">
-        <v>43877</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="3">
-        <v>43878</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="3">
-        <v>43879</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="3">
-        <v>43880</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="3">
-        <v>43881</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="3">
-        <v>43882</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="3">
-        <v>43883</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="3">
-        <v>43884</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="3">
-        <v>43885</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="3">
-        <v>43886</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="3">
-        <v>43887</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="3">
-        <v>43888</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="3">
-        <v>43889</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="3">
-        <v>43890</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="3">
-        <v>43891</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="3">
-        <v>43892</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="3">
-        <v>43893</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="3">
-        <v>43894</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="3">
-        <v>43895</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="3">
-        <v>43896</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="3">
-        <v>43897</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="3">
-        <v>43898</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="3">
-        <v>43899</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="3">
-        <v>43900</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="3">
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="3">
-        <v>43902</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="3">
-        <v>43903</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="3">
-        <v>43904</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="3">
-        <v>43905</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="3">
-        <v>43906</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="3">
-        <v>43907</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="3">
-        <v>43908</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="3">
-        <v>43909</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="3">
-        <v>43910</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="3">
-        <v>43911</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="3">
-        <v>43912</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="3">
-        <v>43913</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="3">
-        <v>43914</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="3">
-        <v>43915</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="3">
-        <v>43916</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="3">
-        <v>43917</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="3">
-        <v>43918</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="3">
-        <v>43919</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="3">
-        <v>43920</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="3">
-        <v>43921</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>